<commit_message>
Implemented all the feedback. Version 2.0
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Subject</t>
   </si>
@@ -124,6 +124,66 @@
   </si>
   <si>
     <t>Making the code readable for everyone.</t>
+  </si>
+  <si>
+    <t>Implenting the scrollview in the about section</t>
+  </si>
+  <si>
+    <t>Added the Scrollview</t>
+  </si>
+  <si>
+    <t>Traits for the homeview</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>Traits for every device for the homeviewcontroller</t>
+  </si>
+  <si>
+    <t>Traits for the aboutview</t>
+  </si>
+  <si>
+    <t>Traits for every device for the aboutview</t>
+  </si>
+  <si>
+    <t>Research Traits</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>I didnt know what this was. So i started to learn how it worked.</t>
+  </si>
+  <si>
+    <t>Traits for the mapview</t>
+  </si>
+  <si>
+    <t>Traits for every device for the mapviewcontroller</t>
+  </si>
+  <si>
+    <t>Appstructure</t>
+  </si>
+  <si>
+    <t>The mapstructure of the app is now better</t>
+  </si>
+  <si>
+    <t>GPS permissions</t>
+  </si>
+  <si>
+    <t>Asking with alertviews for permission of the gps</t>
+  </si>
+  <si>
+    <t>Traits failures</t>
+  </si>
+  <si>
+    <t>The traits didnt worked that well. I needed to set them again for several times.</t>
+  </si>
+  <si>
+    <t>Internet connection</t>
+  </si>
+  <si>
+    <t>I searched and tried to understand what i needed to do. But i didnt know where i needed to check.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +641,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1729,7 +1789,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1921,74 +1981,146 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="19">
+        <v>43089</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="19">
+        <v>43089</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="16"/>
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="19">
+        <v>43089</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="19">
+        <v>43089</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="19">
+        <v>43090</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="19">
+        <v>43090</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="19">
+        <v>43090</v>
+      </c>
+      <c r="C19" s="18">
+        <v>2</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="19">
+        <v>43090</v>
+      </c>
+      <c r="C20" s="18">
+        <v>2</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="19">
+        <v>43090</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
@@ -2062,7 +2194,7 @@
       </c>
       <c r="B30" s="15">
         <f>SUM(C4:C28)</f>
-        <v>9.5</v>
+        <v>14.5</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>

</xml_diff>

<commit_message>
Feedback 2 General is done
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Subject</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>I searched and tried to understand what i needed to do. But i didnt know where i needed to check.</t>
+  </si>
+  <si>
+    <t>App icon + Rotate</t>
+  </si>
+  <si>
+    <t>I improved the app icon. Now it hasn't a black border anymore. And a solved the rotating issue.</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1788,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="159" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2125,10 +2131,18 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="19">
+        <v>43102</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>

</xml_diff>

<commit_message>
added popupadress as subview
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Subject</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Traits for the homeview</t>
   </si>
   <si>
-    <t>1.50</t>
-  </si>
-  <si>
     <t>Traits for every device for the homeviewcontroller</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Research Traits</t>
   </si>
   <si>
-    <t>0.50</t>
-  </si>
-  <si>
     <t>I didnt know what this was. So i started to learn how it worked.</t>
   </si>
   <si>
@@ -196,6 +190,15 @@
   </si>
   <si>
     <t>I implemented the navigationcontroller for all the viewcontrollers</t>
+  </si>
+  <si>
+    <t>Seperated all methods into extentions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I seperated all the methodsd into the correct extentions. </t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="159" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="159" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2010,32 +2013,32 @@
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="19">
         <v>43089</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="19">
         <v>43089</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
@@ -2048,49 +2051,49 @@
         <v>43089</v>
       </c>
       <c r="C16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="19">
         <v>43090</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="19">
         <v>43090</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="19">
         <v>43090</v>
@@ -2099,14 +2102,14 @@
         <v>2</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="19">
         <v>43090</v>
@@ -2115,14 +2118,14 @@
         <v>2</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="19">
         <v>43090</v>
@@ -2131,14 +2134,14 @@
         <v>11</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="19">
         <v>43102</v>
@@ -2147,32 +2150,40 @@
         <v>7</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="19">
         <v>43102</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="19">
+        <v>43103</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>

</xml_diff>

<commit_message>
All the things of feedback 2.0 are done
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Subject</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>Added a subview to the pinView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research pinView </t>
+  </si>
+  <si>
+    <t>I made popupAdress subclassed to pinView. Now the popup will move with the pinView</t>
+  </si>
+  <si>
+    <t>I did research to change the position of the popupAdress while subclassed to the pinView but I couldnt find the solution</t>
   </si>
 </sst>
 </file>
@@ -1803,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="159" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2188,18 +2200,34 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="16"/>
+      <c r="A25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="19">
+        <v>43103</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="16"/>
+      <c r="A26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="19">
+        <v>43103</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="5"/>
     </row>

</xml_diff>